<commit_message>
update merged tasks w/ some jobs, in progress
</commit_message>
<xml_diff>
--- a/tasks/tasks-jobs.xlsx
+++ b/tasks/tasks-jobs.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10723"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julius/work/research/projects/hcml/task-delegability/tasks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bluba\Documents\school\2018-SP\CSCI7000\task-delegability\tasks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{B6D2A06B-FB9A-7840-AAF8-A85DEA8E56C6}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{EF10DA2F-5B84-4412-AFE6-5132DF195758}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51100" windowHeight="28340"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="51105" windowHeight="28335" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tasks-jobs" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="128">
   <si>
     <t>Task</t>
   </si>
@@ -100,18 +100,12 @@
     <t>Editors</t>
   </si>
   <si>
-    <t>Police and Sheriff‚Äôs Patrol Officers</t>
-  </si>
-  <si>
     <t>Travel Agents</t>
   </si>
   <si>
     <t>Chefs and Head Cooks</t>
   </si>
   <si>
-    <t>Hairdressers, Hairstylists, and Cosmetologists</t>
-  </si>
-  <si>
     <t>Air Traffic Controllers</t>
   </si>
   <si>
@@ -347,12 +341,75 @@
   </si>
   <si>
     <t>w</t>
+  </si>
+  <si>
+    <t>Providing support and resources (e.g., develop a treatment plan, provide counseling services and referrals) to individuals to help them recover from mental disorders, similar to what a mental health social worker might do</t>
+  </si>
+  <si>
+    <t>Advising people on nutrition/their diet to help improve their health, similar to what a nutritionist might do</t>
+  </si>
+  <si>
+    <t>Establishing compensation/wage/salary level for an employee</t>
+  </si>
+  <si>
+    <t>Teaching a religion's doctrine and practices to followers, similar to some of the responsibilities of clergy/religious leaders</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Educate patients and their family/friends about various health conditions, similar to a small part of a Registered Nurse's responsibilities </t>
+  </si>
+  <si>
+    <t>For patients with various health conditions, providing advice and emotional support to patients and their family members -- similar to a small part of what a Registered Nurse might do</t>
+  </si>
+  <si>
+    <t>Providing and coordinating patient care in a health facility, similar to a small part of what a Registered Nurse might do.</t>
+  </si>
+  <si>
+    <t>Analyzing, designing, and developing mechanical systems, machines, or devices such as engines or air conditioners -- similar to some of the responsibilities of a mechanical engineer.</t>
+  </si>
+  <si>
+    <t>Designing buildings that meet the needs of the client, and ensure the design meets regulations and building codes, similar to part of what an architect might do</t>
+  </si>
+  <si>
+    <t>Coordinate and oversee construction of a building, e.g., consulting with engineers, surveyors, specialists, and construction workers -- similar to some of what an architect might do.</t>
+  </si>
+  <si>
+    <t>Examining injured or ill patients and developing an individualized plan of care/rehabilitation that promotes movement and healing and reduces pain -- similar to some of what a physical therapist might do.</t>
+  </si>
+  <si>
+    <t>Taking photos of a planned event, such as a wedding or graduation, similar to what a professional photographer might do.</t>
+  </si>
+  <si>
+    <t>Planning and coordinating an event such as a wedding that meets the client's requirements and budget</t>
+  </si>
+  <si>
+    <t>Writing a best-selling mystery novel</t>
+  </si>
+  <si>
+    <t>Planning and supervising farming crop production, including planting, fertilizing, and harvesting -- similar to what a farmer might do</t>
+  </si>
+  <si>
+    <t>Police and Sheriff‚ and Patrol Officers</t>
+  </si>
+  <si>
+    <t>Barbers, Hairstylists, and Cosmetologists</t>
+  </si>
+  <si>
+    <t>Cutting, drying, and styling hair, similar to what a barber or hairstylist might do</t>
+  </si>
+  <si>
+    <t>Planning menus and developing recipes at a restaurant</t>
+  </si>
+  <si>
+    <t>Responding to 911-police incident reports, similar to what a patrol officer might do</t>
+  </si>
+  <si>
+    <t>Coordinate the movement of aircraft to maintain safe distances between them -- similar to what an air traffic controller might do</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1187,19 +1244,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J102"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J105"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B87" sqref="B87"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="60.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1222,7 +1279,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>107</v>
+      </c>
       <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
@@ -1239,7 +1299,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
@@ -1256,7 +1319,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
@@ -1273,7 +1336,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
@@ -1290,7 +1353,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>109</v>
+      </c>
       <c r="B6" s="1" t="s">
         <v>12</v>
       </c>
@@ -1307,7 +1373,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>110</v>
+      </c>
       <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
@@ -1324,7 +1393,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>111</v>
+      </c>
       <c r="B8" s="1" t="s">
         <v>14</v>
       </c>
@@ -1341,172 +1413,189 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="B9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="1">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="E9" s="1">
+        <v>3</v>
+      </c>
+      <c r="F9" s="1">
+        <v>3</v>
+      </c>
+      <c r="G9" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="1">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="E10" s="1">
+        <v>3</v>
+      </c>
+      <c r="F10" s="1">
+        <v>3</v>
+      </c>
+      <c r="G10" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C11" s="1">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="E9" s="1">
-        <v>3</v>
-      </c>
-      <c r="F9" s="1">
-        <v>3</v>
-      </c>
-      <c r="G9" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="1" t="s">
+      <c r="E11" s="1">
+        <v>3</v>
+      </c>
+      <c r="F11" s="1">
+        <v>3</v>
+      </c>
+      <c r="G11" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C12" s="1">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="E10" s="1">
-        <v>3</v>
-      </c>
-      <c r="F10" s="1">
-        <v>3</v>
-      </c>
-      <c r="G10" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="1" t="s">
+      <c r="E12" s="1">
+        <v>3</v>
+      </c>
+      <c r="F12" s="1">
+        <v>3</v>
+      </c>
+      <c r="G12" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C13" s="1">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="E11" s="1">
-        <v>3</v>
-      </c>
-      <c r="F11" s="1">
-        <v>3</v>
-      </c>
-      <c r="G11" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="1" t="s">
+      <c r="E13" s="1">
+        <v>3</v>
+      </c>
+      <c r="F13" s="1">
+        <v>3</v>
+      </c>
+      <c r="G13" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="E14" s="1">
+        <v>3</v>
+      </c>
+      <c r="F14" s="1">
+        <v>3</v>
+      </c>
+      <c r="G14" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C15" s="1">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="E12" s="1">
-        <v>3</v>
-      </c>
-      <c r="F12" s="1">
-        <v>3</v>
-      </c>
-      <c r="G12" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="1" t="s">
+      <c r="E15" s="1">
+        <v>3</v>
+      </c>
+      <c r="F15" s="1">
+        <v>3</v>
+      </c>
+      <c r="G15" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C16" s="1">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="E13" s="1">
-        <v>3</v>
-      </c>
-      <c r="F13" s="1">
-        <v>3</v>
-      </c>
-      <c r="G13" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="1" t="s">
+      <c r="E16" s="1">
+        <v>3</v>
+      </c>
+      <c r="F16" s="1">
+        <v>3</v>
+      </c>
+      <c r="G16" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C17" s="1">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="E14" s="1">
-        <v>3</v>
-      </c>
-      <c r="F14" s="1">
-        <v>3</v>
-      </c>
-      <c r="G14" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1" t="s">
+      <c r="E17" s="1">
+        <v>3</v>
+      </c>
+      <c r="F17" s="1">
+        <v>3</v>
+      </c>
+      <c r="G17" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C18" s="1">
         <v>3.6999999999999998E-2</v>
-      </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1">
-        <v>3</v>
-      </c>
-      <c r="F15" s="1">
-        <v>3</v>
-      </c>
-      <c r="G15" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" s="1">
-        <v>3.7999999999999999E-2</v>
-      </c>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1">
-        <v>3</v>
-      </c>
-      <c r="F16" s="1">
-        <v>3</v>
-      </c>
-      <c r="G16" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="1">
-        <v>4.7E-2</v>
-      </c>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1">
-        <v>3</v>
-      </c>
-      <c r="F17" s="1">
-        <v>3</v>
-      </c>
-      <c r="G17" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" s="1">
-        <v>9.8000000000000004E-2</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1">
@@ -1519,13 +1608,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19" s="1"/>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>120</v>
+      </c>
       <c r="B19" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C19" s="1">
-        <v>0.1</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1">
@@ -1538,13 +1629,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A20" s="1"/>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>121</v>
+      </c>
       <c r="B20" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C20" s="1">
-        <v>0.11</v>
+        <v>4.7E-2</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1">
@@ -1557,13 +1650,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A21" s="1"/>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>126</v>
+      </c>
       <c r="B21" s="1" t="s">
-        <v>30</v>
+        <v>122</v>
       </c>
       <c r="C21" s="1">
-        <v>0.11</v>
+        <v>9.8000000000000004E-2</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1">
@@ -1576,13 +1671,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A22" s="1"/>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>125</v>
+      </c>
       <c r="B22" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C22" s="1">
-        <v>0.13</v>
+        <v>0.1</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1">
@@ -1595,13 +1692,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A23" s="1"/>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>124</v>
+      </c>
       <c r="B23" s="1" t="s">
-        <v>34</v>
+        <v>123</v>
       </c>
       <c r="C23" s="1">
-        <v>0.18</v>
+        <v>0.11</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1">
@@ -1613,17 +1712,16 @@
       <c r="G23" s="1">
         <v>3</v>
       </c>
-      <c r="J23" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A24" s="1"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>127</v>
+      </c>
       <c r="B24" s="1" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="C24" s="1">
-        <v>0.25</v>
+        <v>0.11</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1">
@@ -1636,13 +1734,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="C25" s="1">
-        <v>0.35</v>
+        <v>0.13</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1">
@@ -1655,13 +1753,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="C26" s="1">
-        <v>0.38</v>
+        <v>0.18</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1">
@@ -1673,14 +1771,17 @@
       <c r="G26" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J26" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="C27" s="1">
-        <v>0.4</v>
+        <v>0.25</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1">
@@ -1693,13 +1794,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C28" s="1">
-        <v>0.44</v>
+        <v>0.35</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="1">
@@ -1712,13 +1813,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C29" s="1">
-        <v>0.48</v>
+        <v>0.38</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1">
@@ -1731,13 +1832,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="C30" s="1">
-        <v>0.54</v>
+        <v>0.4</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1">
@@ -1750,13 +1851,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C31" s="1">
-        <v>0.55000000000000004</v>
+        <v>0.44</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1">
@@ -1769,13 +1870,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="C32" s="1">
-        <v>0.63</v>
+        <v>0.48</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1">
@@ -1788,13 +1889,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="C33" s="1">
-        <v>0.66</v>
+        <v>0.54</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="1">
@@ -1807,13 +1908,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="C34" s="1">
-        <v>0.67</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1">
@@ -1826,13 +1927,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="C35" s="1">
-        <v>0.69</v>
+        <v>0.63</v>
       </c>
       <c r="D35" s="1"/>
       <c r="E35" s="1">
@@ -1845,13 +1946,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="C36" s="1">
-        <v>0.69</v>
+        <v>0.66</v>
       </c>
       <c r="D36" s="1"/>
       <c r="E36" s="1">
@@ -1864,13 +1965,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="C37" s="1">
-        <v>0.74</v>
+        <v>0.67</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="1">
@@ -1883,13 +1984,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C38" s="1">
-        <v>0.77</v>
+        <v>0.69</v>
       </c>
       <c r="D38" s="1"/>
       <c r="E38" s="1">
@@ -1902,13 +2003,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C39" s="1">
-        <v>0.8</v>
+        <v>0.69</v>
       </c>
       <c r="D39" s="1"/>
       <c r="E39" s="1">
@@ -1921,13 +2022,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C40" s="1">
-        <v>0.84</v>
+        <v>0.74</v>
       </c>
       <c r="D40" s="1"/>
       <c r="E40" s="1">
@@ -1940,13 +2041,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="C41" s="1">
-        <v>0.84</v>
+        <v>0.77</v>
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="1">
@@ -1959,13 +2060,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="C42" s="1">
-        <v>0.86</v>
+        <v>0.8</v>
       </c>
       <c r="D42" s="1"/>
       <c r="E42" s="1">
@@ -1978,13 +2079,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="1" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C43" s="1">
-        <v>0.86</v>
+        <v>0.84</v>
       </c>
       <c r="D43" s="1"/>
       <c r="E43" s="1">
@@ -1997,13 +2098,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C44" s="1">
-        <v>0.89</v>
+        <v>0.84</v>
       </c>
       <c r="D44" s="1"/>
       <c r="E44" s="1">
@@ -2016,13 +2117,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="C45" s="1">
-        <v>0.9</v>
+        <v>0.86</v>
       </c>
       <c r="D45" s="1"/>
       <c r="E45" s="1">
@@ -2035,13 +2136,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="1" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="C46" s="1">
-        <v>0.91</v>
+        <v>0.86</v>
       </c>
       <c r="D46" s="1"/>
       <c r="E46" s="1">
@@ -2054,13 +2155,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C47" s="1">
-        <v>0.92</v>
+        <v>0.89</v>
       </c>
       <c r="D47" s="1"/>
       <c r="E47" s="1">
@@ -2073,13 +2174,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="1" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="C48" s="1">
-        <v>0.94</v>
+        <v>0.9</v>
       </c>
       <c r="D48" s="1"/>
       <c r="E48" s="1">
@@ -2092,13 +2193,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="1" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="C49" s="1">
-        <v>0.94</v>
+        <v>0.91</v>
       </c>
       <c r="D49" s="1"/>
       <c r="E49" s="1">
@@ -2111,13 +2212,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="1" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="C50" s="1">
-        <v>0.94</v>
+        <v>0.92</v>
       </c>
       <c r="D50" s="1"/>
       <c r="E50" s="1">
@@ -2130,13 +2231,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="1" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="C51" s="1">
-        <v>0.95</v>
+        <v>0.94</v>
       </c>
       <c r="D51" s="1"/>
       <c r="E51" s="1">
@@ -2149,13 +2250,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="1" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="C52" s="1">
-        <v>0.96</v>
+        <v>0.94</v>
       </c>
       <c r="D52" s="1"/>
       <c r="E52" s="1">
@@ -2168,13 +2269,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="1" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="C53" s="1">
-        <v>0.97</v>
+        <v>0.94</v>
       </c>
       <c r="D53" s="1"/>
       <c r="E53" s="1">
@@ -2187,13 +2288,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="1" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="C54" s="1">
-        <v>0.98</v>
+        <v>0.95</v>
       </c>
       <c r="D54" s="1"/>
       <c r="E54" s="1">
@@ -2206,70 +2307,70 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="1" t="s">
-        <v>20</v>
+        <v>95</v>
       </c>
       <c r="C55" s="1">
-        <v>2.8000000000000001E-2</v>
+        <v>0.96</v>
       </c>
       <c r="D55" s="1"/>
       <c r="E55" s="1">
         <v>3</v>
       </c>
       <c r="F55" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G55" s="1">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="1" t="s">
-        <v>27</v>
+        <v>98</v>
       </c>
       <c r="C56" s="1">
-        <v>9.9000000000000005E-2</v>
+        <v>0.97</v>
       </c>
       <c r="D56" s="1"/>
       <c r="E56" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F56" s="1">
         <v>3</v>
       </c>
       <c r="G56" s="1">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="1" t="s">
-        <v>32</v>
+        <v>102</v>
       </c>
       <c r="C57" s="1">
-        <v>0.15</v>
+        <v>0.98</v>
       </c>
       <c r="D57" s="1"/>
       <c r="E57" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F57" s="1">
         <v>3</v>
       </c>
       <c r="G57" s="1">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="1" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="C58" s="1">
-        <v>0.17</v>
+        <v>2.8000000000000001E-2</v>
       </c>
       <c r="D58" s="1"/>
       <c r="E58" s="1">
@@ -2282,51 +2383,51 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="1" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="C59" s="1">
-        <v>0.21</v>
+        <v>9.9000000000000005E-2</v>
       </c>
       <c r="D59" s="1"/>
       <c r="E59" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F59" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G59" s="1">
         <v>2.5</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C60" s="1">
-        <v>0.23</v>
+        <v>0.15</v>
       </c>
       <c r="D60" s="1"/>
       <c r="E60" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F60" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G60" s="1">
         <v>2.5</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C61" s="1">
-        <v>0.25</v>
+        <v>0.17</v>
       </c>
       <c r="D61" s="1"/>
       <c r="E61" s="1">
@@ -2339,13 +2440,13 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C62" s="1">
-        <v>0.35</v>
+        <v>0.21</v>
       </c>
       <c r="D62" s="1"/>
       <c r="E62" s="1">
@@ -2358,13 +2459,13 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="1" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="C63" s="1">
-        <v>0.43</v>
+        <v>0.23</v>
       </c>
       <c r="D63" s="1"/>
       <c r="E63" s="1">
@@ -2377,13 +2478,13 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="1" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="C64" s="1">
-        <v>0.49</v>
+        <v>0.25</v>
       </c>
       <c r="D64" s="1"/>
       <c r="E64" s="1">
@@ -2396,13 +2497,13 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="1" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="C65" s="1">
-        <v>0.5</v>
+        <v>0.35</v>
       </c>
       <c r="D65" s="1"/>
       <c r="E65" s="1">
@@ -2415,13 +2516,13 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C66" s="1">
-        <v>0.53</v>
+        <v>0.43</v>
       </c>
       <c r="D66" s="1"/>
       <c r="E66" s="1">
@@ -2434,13 +2535,13 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C67" s="1">
-        <v>0.56000000000000005</v>
+        <v>0.49</v>
       </c>
       <c r="D67" s="1"/>
       <c r="E67" s="1">
@@ -2453,13 +2554,13 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="C68" s="1">
-        <v>0.59</v>
+        <v>0.5</v>
       </c>
       <c r="D68" s="1"/>
       <c r="E68" s="1">
@@ -2472,13 +2573,13 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="1" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C69" s="1">
-        <v>0.64</v>
+        <v>0.53</v>
       </c>
       <c r="D69" s="1"/>
       <c r="E69" s="1">
@@ -2491,51 +2592,51 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="1" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C70" s="1">
-        <v>0.65</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="D70" s="1"/>
       <c r="E70" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F70" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G70" s="1">
         <v>2.5</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="1" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="C71" s="1">
-        <v>0.67</v>
+        <v>0.59</v>
       </c>
       <c r="D71" s="1"/>
       <c r="E71" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F71" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G71" s="1">
         <v>2.5</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="1" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="C72" s="1">
-        <v>0.68</v>
+        <v>0.64</v>
       </c>
       <c r="D72" s="1"/>
       <c r="E72" s="1">
@@ -2548,51 +2649,51 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="1" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="C73" s="1">
-        <v>0.83</v>
+        <v>0.65</v>
       </c>
       <c r="D73" s="1"/>
       <c r="E73" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F73" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G73" s="1">
         <v>2.5</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="1" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="C74" s="1">
-        <v>0.84</v>
+        <v>0.67</v>
       </c>
       <c r="D74" s="1"/>
       <c r="E74" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F74" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G74" s="1">
         <v>2.5</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="1" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="C75" s="1">
-        <v>0.84</v>
+        <v>0.68</v>
       </c>
       <c r="D75" s="1"/>
       <c r="E75" s="1">
@@ -2605,32 +2706,32 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="1" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="C76" s="1">
-        <v>0.87</v>
+        <v>0.83</v>
       </c>
       <c r="D76" s="1"/>
       <c r="E76" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F76" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G76" s="1">
         <v>2.5</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="1" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C77" s="1">
-        <v>0.89</v>
+        <v>0.84</v>
       </c>
       <c r="D77" s="1"/>
       <c r="E77" s="1">
@@ -2643,13 +2744,13 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="1" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="C78" s="1">
-        <v>0.92</v>
+        <v>0.84</v>
       </c>
       <c r="D78" s="1"/>
       <c r="E78" s="1">
@@ -2662,32 +2763,32 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="1" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="C79" s="1">
-        <v>0.93</v>
+        <v>0.87</v>
       </c>
       <c r="D79" s="1"/>
       <c r="E79" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F79" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G79" s="1">
         <v>2.5</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="1" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="C80" s="1">
-        <v>0.93</v>
+        <v>0.89</v>
       </c>
       <c r="D80" s="1"/>
       <c r="E80" s="1">
@@ -2700,13 +2801,13 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="1" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C81" s="1">
-        <v>0.94</v>
+        <v>0.92</v>
       </c>
       <c r="D81" s="1"/>
       <c r="E81" s="1">
@@ -2719,13 +2820,13 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="1" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="C82" s="1">
-        <v>0.94</v>
+        <v>0.93</v>
       </c>
       <c r="D82" s="1"/>
       <c r="E82" s="1">
@@ -2738,13 +2839,13 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="1" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="C83" s="1">
-        <v>0.96</v>
+        <v>0.93</v>
       </c>
       <c r="D83" s="1"/>
       <c r="E83" s="1">
@@ -2757,13 +2858,13 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84" s="1" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="C84" s="1">
-        <v>0.97</v>
+        <v>0.94</v>
       </c>
       <c r="D84" s="1"/>
       <c r="E84" s="1">
@@ -2776,13 +2877,13 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="1" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="C85" s="1">
-        <v>0.98</v>
+        <v>0.94</v>
       </c>
       <c r="D85" s="1"/>
       <c r="E85" s="1">
@@ -2795,32 +2896,32 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" s="1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C86" s="1">
-        <v>0.98</v>
+        <v>0.96</v>
       </c>
       <c r="D86" s="1"/>
       <c r="E86" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F86" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G86" s="1">
         <v>2.5</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="B87" s="1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="C87" s="1">
-        <v>0.98</v>
+        <v>0.97</v>
       </c>
       <c r="D87" s="1"/>
       <c r="E87" s="1">
@@ -2833,13 +2934,13 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="B88" s="1" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C88" s="1">
-        <v>0.99</v>
+        <v>0.98</v>
       </c>
       <c r="D88" s="1"/>
       <c r="E88" s="1">
@@ -2852,165 +2953,171 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B89" t="s">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A89" s="1"/>
+      <c r="B89" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C89" s="1">
+        <v>0.98</v>
+      </c>
+      <c r="D89" s="1"/>
+      <c r="E89" s="1">
+        <v>2</v>
+      </c>
+      <c r="F89" s="1">
+        <v>3</v>
+      </c>
+      <c r="G89" s="1">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A90" s="1"/>
+      <c r="B90" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C90" s="1">
+        <v>0.98</v>
+      </c>
+      <c r="D90" s="1"/>
+      <c r="E90" s="1">
+        <v>3</v>
+      </c>
+      <c r="F90" s="1">
+        <v>2</v>
+      </c>
+      <c r="G90" s="1">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91" s="1"/>
+      <c r="B91" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C91" s="1">
+        <v>0.99</v>
+      </c>
+      <c r="D91" s="1"/>
+      <c r="E91" s="1">
+        <v>3</v>
+      </c>
+      <c r="F91" s="1">
+        <v>2</v>
+      </c>
+      <c r="G91" s="1">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B92" t="s">
         <v>7</v>
       </c>
-      <c r="C89">
+      <c r="C92">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="E89">
+      <c r="E92">
         <v>1</v>
       </c>
-      <c r="F89">
-        <v>3</v>
-      </c>
-      <c r="G89">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B90" t="s">
+      <c r="F92">
+        <v>3</v>
+      </c>
+      <c r="G92">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B93" t="s">
         <v>25</v>
       </c>
-      <c r="C90">
+      <c r="C93">
         <v>5.5E-2</v>
       </c>
-      <c r="E90">
-        <v>2</v>
-      </c>
-      <c r="F90">
-        <v>2</v>
-      </c>
-      <c r="G90">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B91" t="s">
-        <v>42</v>
-      </c>
-      <c r="C91">
+      <c r="E93">
+        <v>2</v>
+      </c>
+      <c r="F93">
+        <v>2</v>
+      </c>
+      <c r="G93">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B94" t="s">
+        <v>40</v>
+      </c>
+      <c r="C94">
         <v>0.37</v>
       </c>
-      <c r="E91">
-        <v>3</v>
-      </c>
-      <c r="F91">
+      <c r="E94">
+        <v>3</v>
+      </c>
+      <c r="F94">
         <v>1</v>
       </c>
-      <c r="G91">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B92" t="s">
-        <v>54</v>
-      </c>
-      <c r="C92">
+      <c r="G94">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B95" t="s">
+        <v>52</v>
+      </c>
+      <c r="C95">
         <v>0.56999999999999995</v>
       </c>
-      <c r="E92">
-        <v>2</v>
-      </c>
-      <c r="F92">
-        <v>2</v>
-      </c>
-      <c r="G92">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B93" t="s">
-        <v>58</v>
-      </c>
-      <c r="C93">
+      <c r="E95">
+        <v>2</v>
+      </c>
+      <c r="F95">
+        <v>2</v>
+      </c>
+      <c r="G95">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B96" t="s">
+        <v>56</v>
+      </c>
+      <c r="C96">
         <v>0.65</v>
       </c>
-      <c r="E93">
-        <v>2</v>
-      </c>
-      <c r="F93">
-        <v>2</v>
-      </c>
-      <c r="G93">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B94" t="s">
-        <v>64</v>
-      </c>
-      <c r="C94">
+      <c r="E96">
+        <v>2</v>
+      </c>
+      <c r="F96">
+        <v>2</v>
+      </c>
+      <c r="G96">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B97" t="s">
+        <v>62</v>
+      </c>
+      <c r="C97">
         <v>0.68</v>
       </c>
-      <c r="E94">
-        <v>2</v>
-      </c>
-      <c r="F94">
-        <v>2</v>
-      </c>
-      <c r="G94">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B95" t="s">
-        <v>67</v>
-      </c>
-      <c r="C95">
+      <c r="E97">
+        <v>2</v>
+      </c>
+      <c r="F97">
+        <v>2</v>
+      </c>
+      <c r="G97">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="98" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B98" t="s">
+        <v>65</v>
+      </c>
+      <c r="C98">
         <v>0.72</v>
-      </c>
-      <c r="E95">
-        <v>3</v>
-      </c>
-      <c r="F95">
-        <v>1</v>
-      </c>
-      <c r="G95">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B96" t="s">
-        <v>71</v>
-      </c>
-      <c r="C96">
-        <v>0.83</v>
-      </c>
-      <c r="E96">
-        <v>3</v>
-      </c>
-      <c r="F96">
-        <v>1</v>
-      </c>
-      <c r="G96">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="97" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B97" t="s">
-        <v>72</v>
-      </c>
-      <c r="C97">
-        <v>0.83</v>
-      </c>
-      <c r="E97">
-        <v>3</v>
-      </c>
-      <c r="F97">
-        <v>1</v>
-      </c>
-      <c r="G97">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="98" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B98" t="s">
-        <v>95</v>
-      </c>
-      <c r="C98">
-        <v>0.95</v>
       </c>
       <c r="E98">
         <v>3</v>
@@ -3022,12 +3129,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="99" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="99" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
-        <v>98</v>
+        <v>69</v>
       </c>
       <c r="C99">
-        <v>0.96</v>
+        <v>0.83</v>
       </c>
       <c r="E99">
         <v>3</v>
@@ -3039,12 +3146,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="100" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
-        <v>107</v>
+        <v>70</v>
       </c>
       <c r="C100">
-        <v>0.99</v>
+        <v>0.83</v>
       </c>
       <c r="E100">
         <v>3</v>
@@ -3056,42 +3163,93 @@
         <v>2</v>
       </c>
     </row>
-    <row r="101" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
-        <v>39</v>
+        <v>93</v>
       </c>
       <c r="C101">
-        <v>0.28000000000000003</v>
+        <v>0.95</v>
       </c>
       <c r="E101">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F101">
         <v>1</v>
       </c>
       <c r="G101">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="102" spans="2:7" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="C102">
-        <v>0.9</v>
+        <v>0.96</v>
       </c>
       <c r="E102">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F102">
         <v>1</v>
       </c>
       <c r="G102">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="103" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B103" t="s">
+        <v>105</v>
+      </c>
+      <c r="C103">
+        <v>0.99</v>
+      </c>
+      <c r="E103">
+        <v>3</v>
+      </c>
+      <c r="F103">
+        <v>1</v>
+      </c>
+      <c r="G103">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="104" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B104" t="s">
+        <v>37</v>
+      </c>
+      <c r="C104">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="E104">
+        <v>2</v>
+      </c>
+      <c r="F104">
+        <v>1</v>
+      </c>
+      <c r="G104">
         <v>1.5</v>
       </c>
     </row>
+    <row r="105" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B105" t="s">
+        <v>81</v>
+      </c>
+      <c r="C105">
+        <v>0.9</v>
+      </c>
+      <c r="E105">
+        <v>2</v>
+      </c>
+      <c r="F105">
+        <v>1</v>
+      </c>
+      <c r="G105">
+        <v>1.5</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A2:G102">
+  <sortState ref="A2:G105">
     <sortCondition descending="1" ref="G1"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>